<commit_message>
debug ieee39 vsg tds
</commit_message>
<xml_diff>
--- a/bshe/VIS_opf/ieee39_vis.xlsx
+++ b/bshe/VIS_opf/ieee39_vis.xlsx
@@ -2164,7 +2164,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2215,22 +2215,22 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>TGOV1_1</v>
+        <v>TGOV1_2</v>
       </c>
       <c r="C2" t="str">
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <v>TGOV1_1</v>
+        <v>TGOV1_2</v>
       </c>
       <c r="E2" t="str">
-        <v>GENROU_1</v>
+        <v>GENROU_2</v>
       </c>
       <c r="F2" t="str">
-        <v>1040</v>
+        <v>836</v>
       </c>
       <c r="G2" t="str">
         <v>1</v>
@@ -2259,22 +2259,22 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>TGOV1_2</v>
+        <v>TGOV1_3</v>
       </c>
       <c r="C3" t="str">
         <v>1</v>
       </c>
       <c r="D3" t="str">
-        <v>TGOV1_2</v>
+        <v>TGOV1_3</v>
       </c>
       <c r="E3" t="str">
-        <v>GENROU_2</v>
+        <v>GENROU_3</v>
       </c>
       <c r="F3" t="str">
-        <v>836</v>
+        <v>843.7</v>
       </c>
       <c r="G3" t="str">
         <v>1</v>
@@ -2303,22 +2303,22 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>TGOV1_3</v>
+        <v>TGOV1_4</v>
       </c>
       <c r="C4" t="str">
         <v>1</v>
       </c>
       <c r="D4" t="str">
-        <v>TGOV1_3</v>
+        <v>TGOV1_4</v>
       </c>
       <c r="E4" t="str">
-        <v>GENROU_3</v>
+        <v>GENROU_4</v>
       </c>
       <c r="F4" t="str">
-        <v>843.7</v>
+        <v>1174.8</v>
       </c>
       <c r="G4" t="str">
         <v>1</v>
@@ -2347,22 +2347,22 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>TGOV1_4</v>
+        <v>TGOV1_5</v>
       </c>
       <c r="C5" t="str">
         <v>1</v>
       </c>
       <c r="D5" t="str">
-        <v>TGOV1_4</v>
+        <v>TGOV1_5</v>
       </c>
       <c r="E5" t="str">
-        <v>GENROU_4</v>
+        <v>GENROU_5</v>
       </c>
       <c r="F5" t="str">
-        <v>1174.8</v>
+        <v>1080.2</v>
       </c>
       <c r="G5" t="str">
         <v>1</v>
@@ -2391,22 +2391,22 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="str">
-        <v>TGOV1_5</v>
+        <v>TGOV1_7</v>
       </c>
       <c r="C6" t="str">
         <v>1</v>
       </c>
       <c r="D6" t="str">
-        <v>TGOV1_5</v>
+        <v>TGOV1_7</v>
       </c>
       <c r="E6" t="str">
-        <v>GENROU_5</v>
+        <v>GENROU_7</v>
       </c>
       <c r="F6" t="str">
-        <v>1080.2</v>
+        <v>1025.2</v>
       </c>
       <c r="G6" t="str">
         <v>1</v>
@@ -2435,22 +2435,22 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" t="str">
-        <v>TGOV1_6</v>
+        <v>TGOV1_10</v>
       </c>
       <c r="C7" t="str">
         <v>1</v>
       </c>
       <c r="D7" t="str">
-        <v>TGOV1_6</v>
+        <v>TGOV1_10</v>
       </c>
       <c r="E7" t="str">
-        <v>GENROU_6</v>
+        <v>GENROU_10</v>
       </c>
       <c r="F7" t="str">
-        <v>1085.7</v>
+        <v>1199</v>
       </c>
       <c r="G7" t="str">
         <v>1</v>
@@ -2477,192 +2477,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>6</v>
-      </c>
-      <c r="B8" t="str">
-        <v>TGOV1_7</v>
-      </c>
-      <c r="C8" t="str">
-        <v>1</v>
-      </c>
-      <c r="D8" t="str">
-        <v>TGOV1_7</v>
-      </c>
-      <c r="E8" t="str">
-        <v>GENROU_7</v>
-      </c>
-      <c r="F8" t="str">
-        <v>1025.2</v>
-      </c>
-      <c r="G8" t="str">
-        <v>1</v>
-      </c>
-      <c r="H8" t="str">
-        <v>0.05</v>
-      </c>
-      <c r="I8" t="str">
-        <v>1.2</v>
-      </c>
-      <c r="J8" t="str">
-        <v>0</v>
-      </c>
-      <c r="K8" t="str">
-        <v>0.05</v>
-      </c>
-      <c r="L8" t="str">
-        <v>1</v>
-      </c>
-      <c r="M8" t="str">
-        <v>2.1</v>
-      </c>
-      <c r="N8" t="str">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>7</v>
-      </c>
-      <c r="B9" t="str">
-        <v>TGOV1_8</v>
-      </c>
-      <c r="C9" t="str">
-        <v>1</v>
-      </c>
-      <c r="D9" t="str">
-        <v>TGOV1_8</v>
-      </c>
-      <c r="E9" t="str">
-        <v>GENROU_8</v>
-      </c>
-      <c r="F9" t="str">
-        <v>970.2</v>
-      </c>
-      <c r="G9" t="str">
-        <v>1</v>
-      </c>
-      <c r="H9" t="str">
-        <v>0.05</v>
-      </c>
-      <c r="I9" t="str">
-        <v>1.2</v>
-      </c>
-      <c r="J9" t="str">
-        <v>0</v>
-      </c>
-      <c r="K9" t="str">
-        <v>0.05</v>
-      </c>
-      <c r="L9" t="str">
-        <v>1</v>
-      </c>
-      <c r="M9" t="str">
-        <v>2.1</v>
-      </c>
-      <c r="N9" t="str">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>8</v>
-      </c>
-      <c r="B10" t="str">
-        <v>TGOV1_9</v>
-      </c>
-      <c r="C10" t="str">
-        <v>1</v>
-      </c>
-      <c r="D10" t="str">
-        <v>TGOV1_9</v>
-      </c>
-      <c r="E10" t="str">
-        <v>GENROU_9</v>
-      </c>
-      <c r="F10" t="str">
-        <v>1684.1</v>
-      </c>
-      <c r="G10" t="str">
-        <v>1</v>
-      </c>
-      <c r="H10" t="str">
-        <v>0.05</v>
-      </c>
-      <c r="I10" t="str">
-        <v>1.2</v>
-      </c>
-      <c r="J10" t="str">
-        <v>0</v>
-      </c>
-      <c r="K10" t="str">
-        <v>0.05</v>
-      </c>
-      <c r="L10" t="str">
-        <v>1</v>
-      </c>
-      <c r="M10" t="str">
-        <v>2.1</v>
-      </c>
-      <c r="N10" t="str">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>9</v>
-      </c>
-      <c r="B11" t="str">
-        <v>TGOV1_10</v>
-      </c>
-      <c r="C11" t="str">
-        <v>1</v>
-      </c>
-      <c r="D11" t="str">
-        <v>TGOV1_10</v>
-      </c>
-      <c r="E11" t="str">
-        <v>GENROU_10</v>
-      </c>
-      <c r="F11" t="str">
-        <v>1199</v>
-      </c>
-      <c r="G11" t="str">
-        <v>1</v>
-      </c>
-      <c r="H11" t="str">
-        <v>0.05</v>
-      </c>
-      <c r="I11" t="str">
-        <v>1.2</v>
-      </c>
-      <c r="J11" t="str">
-        <v>0</v>
-      </c>
-      <c r="K11" t="str">
-        <v>0.05</v>
-      </c>
-      <c r="L11" t="str">
-        <v>1</v>
-      </c>
-      <c r="M11" t="str">
-        <v>2.1</v>
-      </c>
-      <c r="N11" t="str">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2731,25 +2555,25 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>IEEEX1_1</v>
+        <v>IEEEX1_2</v>
       </c>
       <c r="C2" t="str">
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <v>IEEEX1_1</v>
+        <v>IEEEX1_2</v>
       </c>
       <c r="E2" t="str">
-        <v>GENROU_1</v>
+        <v>GENROU_2</v>
       </c>
       <c r="F2" t="str">
         <v>0</v>
       </c>
       <c r="G2" t="str">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="H2" t="str">
         <v>0</v>
@@ -2758,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="str">
-        <v>0.25</v>
+        <v>0.41</v>
       </c>
       <c r="K2" t="str">
         <v>1.3</v>
@@ -2773,45 +2597,45 @@
         <v>-0.05</v>
       </c>
       <c r="O2" t="str">
-        <v>8</v>
+        <v>5.2</v>
       </c>
       <c r="P2" t="str">
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="Q2" t="str">
-        <v>1.7</v>
+        <v>3</v>
       </c>
       <c r="R2" t="str">
-        <v>0.5</v>
+        <v>0.66</v>
       </c>
       <c r="S2" t="str">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T2" t="str">
-        <v>2</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>IEEEX1_2</v>
+        <v>IEEEX1_3</v>
       </c>
       <c r="C3" t="str">
         <v>1</v>
       </c>
       <c r="D3" t="str">
-        <v>IEEEX1_2</v>
+        <v>IEEEX1_3</v>
       </c>
       <c r="E3" t="str">
-        <v>GENROU_2</v>
+        <v>GENROU_3</v>
       </c>
       <c r="F3" t="str">
         <v>0</v>
       </c>
       <c r="G3" t="str">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="H3" t="str">
         <v>0</v>
@@ -2820,7 +2644,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="str">
-        <v>0.41</v>
+        <v>0.5</v>
       </c>
       <c r="K3" t="str">
         <v>1.3</v>
@@ -2832,10 +2656,10 @@
         <v>10.1</v>
       </c>
       <c r="N3" t="str">
-        <v>-0.05</v>
+        <v>-0.02</v>
       </c>
       <c r="O3" t="str">
-        <v>5.2</v>
+        <v>5</v>
       </c>
       <c r="P3" t="str">
         <v>-5</v>
@@ -2844,30 +2668,30 @@
         <v>3</v>
       </c>
       <c r="R3" t="str">
-        <v>0.66</v>
+        <v>0.13</v>
       </c>
       <c r="S3" t="str">
         <v>4</v>
       </c>
       <c r="T3" t="str">
-        <v>0.88</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>IEEEX1_3</v>
+        <v>IEEEX1_4</v>
       </c>
       <c r="C4" t="str">
         <v>1</v>
       </c>
       <c r="D4" t="str">
-        <v>IEEEX1_3</v>
+        <v>IEEEX1_4</v>
       </c>
       <c r="E4" t="str">
-        <v>GENROU_3</v>
+        <v>GENROU_4</v>
       </c>
       <c r="F4" t="str">
         <v>0</v>
@@ -2894,7 +2718,7 @@
         <v>10.1</v>
       </c>
       <c r="N4" t="str">
-        <v>-0.02</v>
+        <v>-0.05</v>
       </c>
       <c r="O4" t="str">
         <v>5</v>
@@ -2906,36 +2730,36 @@
         <v>3</v>
       </c>
       <c r="R4" t="str">
-        <v>0.13</v>
+        <v>0.08</v>
       </c>
       <c r="S4" t="str">
         <v>4</v>
       </c>
       <c r="T4" t="str">
-        <v>0.34</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>IEEEX1_4</v>
+        <v>IEEEX1_5</v>
       </c>
       <c r="C5" t="str">
         <v>1</v>
       </c>
       <c r="D5" t="str">
-        <v>IEEEX1_4</v>
+        <v>IEEEX1_5</v>
       </c>
       <c r="E5" t="str">
-        <v>GENROU_4</v>
+        <v>GENROU_5</v>
       </c>
       <c r="F5" t="str">
         <v>0</v>
       </c>
       <c r="G5" t="str">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="H5" t="str">
         <v>0</v>
@@ -2944,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="str">
-        <v>0.5</v>
+        <v>0.785</v>
       </c>
       <c r="K5" t="str">
         <v>1.3</v>
@@ -2953,45 +2777,45 @@
         <v>0.23</v>
       </c>
       <c r="M5" t="str">
-        <v>10.1</v>
+        <v>40</v>
       </c>
       <c r="N5" t="str">
-        <v>-0.05</v>
+        <v>-0.04</v>
       </c>
       <c r="O5" t="str">
-        <v>5</v>
+        <v>9.9</v>
       </c>
       <c r="P5" t="str">
-        <v>-5</v>
+        <v>-9.9</v>
       </c>
       <c r="Q5" t="str">
         <v>3</v>
       </c>
       <c r="R5" t="str">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="S5" t="str">
         <v>4</v>
       </c>
       <c r="T5" t="str">
-        <v>0.31</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="str">
-        <v>IEEEX1_5</v>
+        <v>IEEEX1_7</v>
       </c>
       <c r="C6" t="str">
         <v>1</v>
       </c>
       <c r="D6" t="str">
-        <v>IEEEX1_5</v>
+        <v>IEEEX1_7</v>
       </c>
       <c r="E6" t="str">
-        <v>GENROU_5</v>
+        <v>GENROU_7</v>
       </c>
       <c r="F6" t="str">
         <v>0</v>
@@ -3006,7 +2830,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="str">
-        <v>0.785</v>
+        <v>0.73</v>
       </c>
       <c r="K6" t="str">
         <v>1.3</v>
@@ -3018,13 +2842,13 @@
         <v>40</v>
       </c>
       <c r="N6" t="str">
-        <v>-0.04</v>
+        <v>1</v>
       </c>
       <c r="O6" t="str">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="P6" t="str">
-        <v>-9.9</v>
+        <v>-6.5</v>
       </c>
       <c r="Q6" t="str">
         <v>3</v>
@@ -3036,24 +2860,24 @@
         <v>4</v>
       </c>
       <c r="T6" t="str">
-        <v>0.91</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" t="str">
-        <v>IEEEX1_6</v>
+        <v>IEEEX1_10</v>
       </c>
       <c r="C7" t="str">
         <v>1</v>
       </c>
       <c r="D7" t="str">
-        <v>IEEEX1_6</v>
+        <v>IEEEX1_10</v>
       </c>
       <c r="E7" t="str">
-        <v>GENROU_6</v>
+        <v>GENROU_10</v>
       </c>
       <c r="F7" t="str">
         <v>0</v>
@@ -3068,7 +2892,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="str">
-        <v>0.471</v>
+        <v>0.95</v>
       </c>
       <c r="K7" t="str">
         <v>1.3</v>
@@ -3083,282 +2907,34 @@
         <v>1</v>
       </c>
       <c r="O7" t="str">
-        <v>5</v>
+        <v>9.9</v>
       </c>
       <c r="P7" t="str">
-        <v>-5</v>
+        <v>-9.9</v>
       </c>
       <c r="Q7" t="str">
         <v>3</v>
       </c>
       <c r="R7" t="str">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="S7" t="str">
         <v>4</v>
       </c>
       <c r="T7" t="str">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>6</v>
-      </c>
-      <c r="B8" t="str">
-        <v>IEEEX1_7</v>
-      </c>
-      <c r="C8" t="str">
-        <v>1</v>
-      </c>
-      <c r="D8" t="str">
-        <v>IEEEX1_7</v>
-      </c>
-      <c r="E8" t="str">
-        <v>GENROU_7</v>
-      </c>
-      <c r="F8" t="str">
-        <v>0</v>
-      </c>
-      <c r="G8" t="str">
-        <v>0.02</v>
-      </c>
-      <c r="H8" t="str">
-        <v>0</v>
-      </c>
-      <c r="I8" t="str">
-        <v>0</v>
-      </c>
-      <c r="J8" t="str">
-        <v>0.73</v>
-      </c>
-      <c r="K8" t="str">
-        <v>1.3</v>
-      </c>
-      <c r="L8" t="str">
-        <v>0.23</v>
-      </c>
-      <c r="M8" t="str">
-        <v>40</v>
-      </c>
-      <c r="N8" t="str">
-        <v>1</v>
-      </c>
-      <c r="O8" t="str">
-        <v>6.5</v>
-      </c>
-      <c r="P8" t="str">
-        <v>-6.5</v>
-      </c>
-      <c r="Q8" t="str">
-        <v>3</v>
-      </c>
-      <c r="R8" t="str">
-        <v>0.03</v>
-      </c>
-      <c r="S8" t="str">
-        <v>4</v>
-      </c>
-      <c r="T8" t="str">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>7</v>
-      </c>
-      <c r="B9" t="str">
-        <v>IEEEX1_8</v>
-      </c>
-      <c r="C9" t="str">
-        <v>1</v>
-      </c>
-      <c r="D9" t="str">
-        <v>IEEEX1_8</v>
-      </c>
-      <c r="E9" t="str">
-        <v>GENROU_8</v>
-      </c>
-      <c r="F9" t="str">
-        <v>0</v>
-      </c>
-      <c r="G9" t="str">
-        <v>0.02</v>
-      </c>
-      <c r="H9" t="str">
-        <v>0</v>
-      </c>
-      <c r="I9" t="str">
-        <v>0</v>
-      </c>
-      <c r="J9" t="str">
-        <v>0.528</v>
-      </c>
-      <c r="K9" t="str">
-        <v>1.3</v>
-      </c>
-      <c r="L9" t="str">
-        <v>0.23</v>
-      </c>
-      <c r="M9" t="str">
-        <v>10.1</v>
-      </c>
-      <c r="N9" t="str">
-        <v>-0.05</v>
-      </c>
-      <c r="O9" t="str">
-        <v>5</v>
-      </c>
-      <c r="P9" t="str">
-        <v>-5</v>
-      </c>
-      <c r="Q9" t="str">
-        <v>3</v>
-      </c>
-      <c r="R9" t="str">
-        <v>0.09</v>
-      </c>
-      <c r="S9" t="str">
-        <v>4</v>
-      </c>
-      <c r="T9" t="str">
-        <v>0.28</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>8</v>
-      </c>
-      <c r="B10" t="str">
-        <v>IEEEX1_9</v>
-      </c>
-      <c r="C10" t="str">
-        <v>1</v>
-      </c>
-      <c r="D10" t="str">
-        <v>IEEEX1_9</v>
-      </c>
-      <c r="E10" t="str">
-        <v>GENROU_9</v>
-      </c>
-      <c r="F10" t="str">
-        <v>0</v>
-      </c>
-      <c r="G10" t="str">
-        <v>0.02</v>
-      </c>
-      <c r="H10" t="str">
-        <v>0</v>
-      </c>
-      <c r="I10" t="str">
-        <v>0</v>
-      </c>
-      <c r="J10" t="str">
-        <v>0.95</v>
-      </c>
-      <c r="K10" t="str">
-        <v>1.3</v>
-      </c>
-      <c r="L10" t="str">
-        <v>0.23</v>
-      </c>
-      <c r="M10" t="str">
-        <v>40</v>
-      </c>
-      <c r="N10" t="str">
-        <v>1</v>
-      </c>
-      <c r="O10" t="str">
-        <v>9.9</v>
-      </c>
-      <c r="P10" t="str">
-        <v>-9.9</v>
-      </c>
-      <c r="Q10" t="str">
-        <v>3</v>
-      </c>
-      <c r="R10" t="str">
-        <v>0.03</v>
-      </c>
-      <c r="S10" t="str">
-        <v>4</v>
-      </c>
-      <c r="T10" t="str">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>9</v>
-      </c>
-      <c r="B11" t="str">
-        <v>IEEEX1_10</v>
-      </c>
-      <c r="C11" t="str">
-        <v>1</v>
-      </c>
-      <c r="D11" t="str">
-        <v>IEEEX1_10</v>
-      </c>
-      <c r="E11" t="str">
-        <v>GENROU_10</v>
-      </c>
-      <c r="F11" t="str">
-        <v>0</v>
-      </c>
-      <c r="G11" t="str">
-        <v>0.02</v>
-      </c>
-      <c r="H11" t="str">
-        <v>0</v>
-      </c>
-      <c r="I11" t="str">
-        <v>0</v>
-      </c>
-      <c r="J11" t="str">
-        <v>0.95</v>
-      </c>
-      <c r="K11" t="str">
-        <v>1.3</v>
-      </c>
-      <c r="L11" t="str">
-        <v>0.23</v>
-      </c>
-      <c r="M11" t="str">
-        <v>10.1</v>
-      </c>
-      <c r="N11" t="str">
-        <v>1</v>
-      </c>
-      <c r="O11" t="str">
-        <v>9.9</v>
-      </c>
-      <c r="P11" t="str">
-        <v>-9.9</v>
-      </c>
-      <c r="Q11" t="str">
-        <v>3</v>
-      </c>
-      <c r="R11" t="str">
-        <v>0.03</v>
-      </c>
-      <c r="S11" t="str">
-        <v>4</v>
-      </c>
-      <c r="T11" t="str">
         <v>0.85</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:T11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3442,25 +3018,25 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>IEEEST_1</v>
+        <v>IEEEST_2</v>
       </c>
       <c r="C2" t="str">
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <v>IEEEST_1</v>
+        <v>IEEEST_2</v>
       </c>
       <c r="E2" t="str">
-        <v>IEEEX1_1</v>
+        <v>IEEEX1_2</v>
       </c>
       <c r="F2" t="str">
         <v>3</v>
       </c>
       <c r="H2" t="str">
-        <v>BusFreq_1</v>
+        <v>BusFreq_2</v>
       </c>
       <c r="I2" t="str">
         <v>0</v>
@@ -3516,25 +3092,25 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>IEEEST_2</v>
+        <v>IEEEST_3</v>
       </c>
       <c r="C3" t="str">
         <v>1</v>
       </c>
       <c r="D3" t="str">
-        <v>IEEEST_2</v>
+        <v>IEEEST_3</v>
       </c>
       <c r="E3" t="str">
-        <v>IEEEX1_2</v>
+        <v>IEEEX1_3</v>
       </c>
       <c r="F3" t="str">
         <v>3</v>
       </c>
       <c r="H3" t="str">
-        <v>BusFreq_2</v>
+        <v>BusFreq_3</v>
       </c>
       <c r="I3" t="str">
         <v>0</v>
@@ -3590,25 +3166,25 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>IEEEST_3</v>
+        <v>IEEEST_4</v>
       </c>
       <c r="C4" t="str">
         <v>1</v>
       </c>
       <c r="D4" t="str">
-        <v>IEEEST_3</v>
+        <v>IEEEST_4</v>
       </c>
       <c r="E4" t="str">
-        <v>IEEEX1_3</v>
+        <v>IEEEX1_4</v>
       </c>
       <c r="F4" t="str">
         <v>3</v>
       </c>
       <c r="H4" t="str">
-        <v>BusFreq_3</v>
+        <v>BusFreq_4</v>
       </c>
       <c r="I4" t="str">
         <v>0</v>
@@ -3664,25 +3240,25 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>IEEEST_4</v>
+        <v>IEEEST_5</v>
       </c>
       <c r="C5" t="str">
         <v>1</v>
       </c>
       <c r="D5" t="str">
-        <v>IEEEST_4</v>
+        <v>IEEEST_5</v>
       </c>
       <c r="E5" t="str">
-        <v>IEEEX1_4</v>
+        <v>IEEEX1_5</v>
       </c>
       <c r="F5" t="str">
         <v>3</v>
       </c>
       <c r="H5" t="str">
-        <v>BusFreq_4</v>
+        <v>BusFreq_5</v>
       </c>
       <c r="I5" t="str">
         <v>0</v>
@@ -3738,25 +3314,25 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="str">
-        <v>IEEEST_5</v>
+        <v>IEEEST_7</v>
       </c>
       <c r="C6" t="str">
         <v>1</v>
       </c>
       <c r="D6" t="str">
-        <v>IEEEST_5</v>
+        <v>IEEEST_7</v>
       </c>
       <c r="E6" t="str">
-        <v>IEEEX1_5</v>
+        <v>IEEEX1_7</v>
       </c>
       <c r="F6" t="str">
         <v>3</v>
       </c>
       <c r="H6" t="str">
-        <v>BusFreq_5</v>
+        <v>BusFreq_7</v>
       </c>
       <c r="I6" t="str">
         <v>0</v>
@@ -3812,25 +3388,25 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" t="str">
-        <v>IEEEST_6</v>
+        <v>IEEEST_10</v>
       </c>
       <c r="C7" t="str">
         <v>1</v>
       </c>
       <c r="D7" t="str">
-        <v>IEEEST_6</v>
+        <v>IEEEST_10</v>
       </c>
       <c r="E7" t="str">
-        <v>IEEEX1_6</v>
+        <v>IEEEX1_10</v>
       </c>
       <c r="F7" t="str">
         <v>3</v>
       </c>
       <c r="H7" t="str">
-        <v>BusFreq_6</v>
+        <v>BusFreq_10</v>
       </c>
       <c r="I7" t="str">
         <v>0</v>
@@ -3884,305 +3460,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>6</v>
-      </c>
-      <c r="B8" t="str">
-        <v>IEEEST_7</v>
-      </c>
-      <c r="C8" t="str">
-        <v>1</v>
-      </c>
-      <c r="D8" t="str">
-        <v>IEEEST_7</v>
-      </c>
-      <c r="E8" t="str">
-        <v>IEEEX1_7</v>
-      </c>
-      <c r="F8" t="str">
-        <v>3</v>
-      </c>
-      <c r="H8" t="str">
-        <v>BusFreq_7</v>
-      </c>
-      <c r="I8" t="str">
-        <v>0</v>
-      </c>
-      <c r="J8" t="str">
-        <v>0</v>
-      </c>
-      <c r="K8" t="str">
-        <v>0</v>
-      </c>
-      <c r="L8" t="str">
-        <v>0</v>
-      </c>
-      <c r="M8" t="str">
-        <v>0</v>
-      </c>
-      <c r="N8" t="str">
-        <v>0</v>
-      </c>
-      <c r="O8" t="str">
-        <v>0</v>
-      </c>
-      <c r="P8" t="str">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="str">
-        <v>0</v>
-      </c>
-      <c r="R8" t="str">
-        <v>0.75</v>
-      </c>
-      <c r="S8" t="str">
-        <v>1</v>
-      </c>
-      <c r="T8" t="str">
-        <v>4.2</v>
-      </c>
-      <c r="U8" t="str">
-        <v>-2</v>
-      </c>
-      <c r="V8" t="str">
-        <v>0.1</v>
-      </c>
-      <c r="W8" t="str">
-        <v>-0.1</v>
-      </c>
-      <c r="X8" t="str">
-        <v>0</v>
-      </c>
-      <c r="Y8" t="str">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>7</v>
-      </c>
-      <c r="B9" t="str">
-        <v>IEEEST_8</v>
-      </c>
-      <c r="C9" t="str">
-        <v>1</v>
-      </c>
-      <c r="D9" t="str">
-        <v>IEEEST_8</v>
-      </c>
-      <c r="E9" t="str">
-        <v>IEEEX1_8</v>
-      </c>
-      <c r="F9" t="str">
-        <v>3</v>
-      </c>
-      <c r="H9" t="str">
-        <v>BusFreq_8</v>
-      </c>
-      <c r="I9" t="str">
-        <v>0</v>
-      </c>
-      <c r="J9" t="str">
-        <v>0</v>
-      </c>
-      <c r="K9" t="str">
-        <v>0</v>
-      </c>
-      <c r="L9" t="str">
-        <v>0</v>
-      </c>
-      <c r="M9" t="str">
-        <v>0</v>
-      </c>
-      <c r="N9" t="str">
-        <v>0</v>
-      </c>
-      <c r="O9" t="str">
-        <v>0</v>
-      </c>
-      <c r="P9" t="str">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="str">
-        <v>0</v>
-      </c>
-      <c r="R9" t="str">
-        <v>0.75</v>
-      </c>
-      <c r="S9" t="str">
-        <v>1</v>
-      </c>
-      <c r="T9" t="str">
-        <v>4.2</v>
-      </c>
-      <c r="U9" t="str">
-        <v>-2</v>
-      </c>
-      <c r="V9" t="str">
-        <v>0.1</v>
-      </c>
-      <c r="W9" t="str">
-        <v>-0.1</v>
-      </c>
-      <c r="X9" t="str">
-        <v>0</v>
-      </c>
-      <c r="Y9" t="str">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>8</v>
-      </c>
-      <c r="B10" t="str">
-        <v>IEEEST_9</v>
-      </c>
-      <c r="C10" t="str">
-        <v>1</v>
-      </c>
-      <c r="D10" t="str">
-        <v>IEEEST_9</v>
-      </c>
-      <c r="E10" t="str">
-        <v>IEEEX1_9</v>
-      </c>
-      <c r="F10" t="str">
-        <v>3</v>
-      </c>
-      <c r="H10" t="str">
-        <v>BusFreq_9</v>
-      </c>
-      <c r="I10" t="str">
-        <v>0</v>
-      </c>
-      <c r="J10" t="str">
-        <v>0</v>
-      </c>
-      <c r="K10" t="str">
-        <v>0</v>
-      </c>
-      <c r="L10" t="str">
-        <v>0</v>
-      </c>
-      <c r="M10" t="str">
-        <v>0</v>
-      </c>
-      <c r="N10" t="str">
-        <v>0</v>
-      </c>
-      <c r="O10" t="str">
-        <v>0</v>
-      </c>
-      <c r="P10" t="str">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="str">
-        <v>0</v>
-      </c>
-      <c r="R10" t="str">
-        <v>0.75</v>
-      </c>
-      <c r="S10" t="str">
-        <v>1</v>
-      </c>
-      <c r="T10" t="str">
-        <v>4.2</v>
-      </c>
-      <c r="U10" t="str">
-        <v>-2</v>
-      </c>
-      <c r="V10" t="str">
-        <v>0.1</v>
-      </c>
-      <c r="W10" t="str">
-        <v>-0.1</v>
-      </c>
-      <c r="X10" t="str">
-        <v>0</v>
-      </c>
-      <c r="Y10" t="str">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>9</v>
-      </c>
-      <c r="B11" t="str">
-        <v>IEEEST_10</v>
-      </c>
-      <c r="C11" t="str">
-        <v>1</v>
-      </c>
-      <c r="D11" t="str">
-        <v>IEEEST_10</v>
-      </c>
-      <c r="E11" t="str">
-        <v>IEEEX1_10</v>
-      </c>
-      <c r="F11" t="str">
-        <v>3</v>
-      </c>
-      <c r="H11" t="str">
-        <v>BusFreq_10</v>
-      </c>
-      <c r="I11" t="str">
-        <v>0</v>
-      </c>
-      <c r="J11" t="str">
-        <v>0</v>
-      </c>
-      <c r="K11" t="str">
-        <v>0</v>
-      </c>
-      <c r="L11" t="str">
-        <v>0</v>
-      </c>
-      <c r="M11" t="str">
-        <v>0</v>
-      </c>
-      <c r="N11" t="str">
-        <v>0</v>
-      </c>
-      <c r="O11" t="str">
-        <v>0</v>
-      </c>
-      <c r="P11" t="str">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="str">
-        <v>0</v>
-      </c>
-      <c r="R11" t="str">
-        <v>0.75</v>
-      </c>
-      <c r="S11" t="str">
-        <v>1</v>
-      </c>
-      <c r="T11" t="str">
-        <v>4.2</v>
-      </c>
-      <c r="U11" t="str">
-        <v>-2</v>
-      </c>
-      <c r="V11" t="str">
-        <v>0.1</v>
-      </c>
-      <c r="W11" t="str">
-        <v>-0.1</v>
-      </c>
-      <c r="X11" t="str">
-        <v>0</v>
-      </c>
-      <c r="Y11" t="str">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Y11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Y7"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4549,7 +3829,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4594,15 +3874,43 @@
         <v>GENROU</v>
       </c>
       <c r="F2" t="str">
-        <v>GENROU_1</v>
+        <v>GENROU_2</v>
       </c>
       <c r="G2" t="str">
-        <v>12</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Toggler_2</v>
+      </c>
+      <c r="C3" t="str">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Toggler_1</v>
+      </c>
+      <c r="E3" t="str">
+        <v>PQ</v>
+      </c>
+      <c r="F3" t="str">
+        <v>PQ_20</v>
+      </c>
+      <c r="G3" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="E6" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4651,7 +3959,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5356,9 +4664,44 @@
         <v>1</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>19</v>
+      </c>
+      <c r="B21" t="str">
+        <v>PQ_20</v>
+      </c>
+      <c r="C21" t="str">
+        <v>0</v>
+      </c>
+      <c r="D21" t="str">
+        <v>PQ_18</v>
+      </c>
+      <c r="E21" t="str">
+        <v>31</v>
+      </c>
+      <c r="F21" t="str">
+        <v>34.5</v>
+      </c>
+      <c r="G21" t="str">
+        <v>0.8</v>
+      </c>
+      <c r="H21" t="str">
+        <v>0.4</v>
+      </c>
+      <c r="I21" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="J21" t="str">
+        <v>0.8</v>
+      </c>
+      <c r="K21" t="str">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K21"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9744,7 +9087,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9837,28 +9180,28 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>GENROU_1</v>
+        <v>GENROU_2</v>
       </c>
       <c r="C2" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="str">
-        <v>GENROU_1</v>
+        <v>GENROU_2</v>
       </c>
       <c r="E2" t="str">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F2" t="str">
-        <v>PV_1</v>
+        <v>PV_2</v>
       </c>
       <c r="G2" t="str">
         <v>COI_1</v>
       </c>
       <c r="H2" t="str">
-        <v>1040</v>
+        <v>836</v>
       </c>
       <c r="I2" t="str">
         <v>34.5</v>
@@ -9870,16 +9213,16 @@
         <v>0</v>
       </c>
       <c r="L2" t="str">
-        <v>8.4</v>
+        <v>8.06</v>
       </c>
       <c r="M2" t="str">
-        <v>0.0014</v>
+        <v>0.027</v>
       </c>
       <c r="N2" t="str">
-        <v>0.125</v>
+        <v>0.35</v>
       </c>
       <c r="O2" t="str">
-        <v>0.31</v>
+        <v>0.697</v>
       </c>
       <c r="P2" t="str">
         <v>0</v>
@@ -9894,22 +9237,22 @@
         <v>0</v>
       </c>
       <c r="T2" t="str">
-        <v>1</v>
+        <v>2.95</v>
       </c>
       <c r="U2" t="str">
-        <v>0.69</v>
+        <v>2.82</v>
       </c>
       <c r="V2" t="str">
-        <v>0.00792</v>
+        <v>0.29779</v>
       </c>
       <c r="W2" t="str">
-        <v>0.31</v>
+        <v>0.697</v>
       </c>
       <c r="X2" t="str">
-        <v>0.00792</v>
+        <v>0.29779</v>
       </c>
       <c r="Y2" t="str">
-        <v>10.2</v>
+        <v>6.56</v>
       </c>
       <c r="Z2" t="str">
         <v>0.03</v>
@@ -9923,31 +9266,31 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>GENROU_2</v>
+        <v>GENROU_3</v>
       </c>
       <c r="C3" t="str">
         <v>1</v>
       </c>
       <c r="D3" t="str">
-        <v>GENROU_2</v>
+        <v>GENROU_3</v>
       </c>
       <c r="E3" t="str">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F3" t="str">
-        <v>PV_2</v>
+        <v>PV_3</v>
       </c>
       <c r="G3" t="str">
         <v>COI_1</v>
       </c>
       <c r="H3" t="str">
-        <v>836</v>
+        <v>843.7</v>
       </c>
       <c r="I3" t="str">
-        <v>34.5</v>
+        <v>21</v>
       </c>
       <c r="J3" t="str">
         <v>60</v>
@@ -9956,16 +9299,16 @@
         <v>0</v>
       </c>
       <c r="L3" t="str">
-        <v>6.06</v>
+        <v>7.16</v>
       </c>
       <c r="M3" t="str">
-        <v>0.027</v>
+        <v>0.00386</v>
       </c>
       <c r="N3" t="str">
-        <v>0.35</v>
+        <v>0.304</v>
       </c>
       <c r="O3" t="str">
-        <v>0.697</v>
+        <v>0.531</v>
       </c>
       <c r="P3" t="str">
         <v>0</v>
@@ -9980,22 +9323,22 @@
         <v>0</v>
       </c>
       <c r="T3" t="str">
-        <v>2.95</v>
+        <v>2.495</v>
       </c>
       <c r="U3" t="str">
-        <v>2.82</v>
+        <v>2.37</v>
       </c>
       <c r="V3" t="str">
-        <v>0.29779</v>
+        <v>0.02566</v>
       </c>
       <c r="W3" t="str">
-        <v>0.697</v>
+        <v>0.531</v>
       </c>
       <c r="X3" t="str">
-        <v>0.29779</v>
+        <v>0.02566</v>
       </c>
       <c r="Y3" t="str">
-        <v>6.56</v>
+        <v>5.7</v>
       </c>
       <c r="Z3" t="str">
         <v>0.03</v>
@@ -10009,28 +9352,28 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>GENROU_3</v>
+        <v>GENROU_4</v>
       </c>
       <c r="C4" t="str">
         <v>1</v>
       </c>
       <c r="D4" t="str">
-        <v>GENROU_3</v>
+        <v>GENROU_4</v>
       </c>
       <c r="E4" t="str">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" t="str">
-        <v>PV_3</v>
+        <v>PV_4</v>
       </c>
       <c r="G4" t="str">
         <v>COI_1</v>
       </c>
       <c r="H4" t="str">
-        <v>843.7</v>
+        <v>1174.8</v>
       </c>
       <c r="I4" t="str">
         <v>21</v>
@@ -10042,16 +9385,16 @@
         <v>0</v>
       </c>
       <c r="L4" t="str">
-        <v>7.16</v>
+        <v>8.72</v>
       </c>
       <c r="M4" t="str">
-        <v>0.00386</v>
+        <v>0.00222</v>
       </c>
       <c r="N4" t="str">
-        <v>0.304</v>
+        <v>0.295</v>
       </c>
       <c r="O4" t="str">
-        <v>0.531</v>
+        <v>0.436</v>
       </c>
       <c r="P4" t="str">
         <v>0</v>
@@ -10066,22 +9409,22 @@
         <v>0</v>
       </c>
       <c r="T4" t="str">
-        <v>2.495</v>
+        <v>2.62</v>
       </c>
       <c r="U4" t="str">
-        <v>2.37</v>
+        <v>2.58</v>
       </c>
       <c r="V4" t="str">
-        <v>0.02566</v>
+        <v>0.00803</v>
       </c>
       <c r="W4" t="str">
-        <v>0.531</v>
+        <v>0.436</v>
       </c>
       <c r="X4" t="str">
-        <v>0.02566</v>
+        <v>0.00803</v>
       </c>
       <c r="Y4" t="str">
-        <v>5.7</v>
+        <v>5.69</v>
       </c>
       <c r="Z4" t="str">
         <v>0.03</v>
@@ -10095,31 +9438,31 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>GENROU_4</v>
+        <v>GENROU_5</v>
       </c>
       <c r="C5" t="str">
         <v>1</v>
       </c>
       <c r="D5" t="str">
-        <v>GENROU_4</v>
+        <v>GENROU_5</v>
       </c>
       <c r="E5" t="str">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" t="str">
-        <v>PV_4</v>
+        <v>PV_5</v>
       </c>
       <c r="G5" t="str">
         <v>COI_1</v>
       </c>
       <c r="H5" t="str">
-        <v>1174.8</v>
+        <v>1080.2</v>
       </c>
       <c r="I5" t="str">
-        <v>21</v>
+        <v>15.5</v>
       </c>
       <c r="J5" t="str">
         <v>60</v>
@@ -10128,16 +9471,16 @@
         <v>0</v>
       </c>
       <c r="L5" t="str">
-        <v>5.72</v>
+        <v>5.2</v>
       </c>
       <c r="M5" t="str">
-        <v>0.00222</v>
+        <v>0.0014</v>
       </c>
       <c r="N5" t="str">
-        <v>0.295</v>
+        <v>0.54</v>
       </c>
       <c r="O5" t="str">
-        <v>0.436</v>
+        <v>1.32</v>
       </c>
       <c r="P5" t="str">
         <v>0</v>
@@ -10152,28 +9495,28 @@
         <v>0</v>
       </c>
       <c r="T5" t="str">
-        <v>2.62</v>
+        <v>6.7</v>
       </c>
       <c r="U5" t="str">
-        <v>2.58</v>
+        <v>6.2</v>
       </c>
       <c r="V5" t="str">
-        <v>0.00803</v>
+        <v>0.00571</v>
       </c>
       <c r="W5" t="str">
-        <v>0.436</v>
+        <v>1.32</v>
       </c>
       <c r="X5" t="str">
-        <v>0.00803</v>
+        <v>0.00571</v>
       </c>
       <c r="Y5" t="str">
-        <v>5.69</v>
+        <v>5.4</v>
       </c>
       <c r="Z5" t="str">
         <v>0.03</v>
       </c>
       <c r="AA5" t="str">
-        <v>1.5</v>
+        <v>0.44</v>
       </c>
       <c r="AB5" t="str">
         <v>0.04</v>
@@ -10181,31 +9524,31 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="str">
-        <v>GENROU_5</v>
+        <v>GENROU_7</v>
       </c>
       <c r="C6" t="str">
         <v>1</v>
       </c>
       <c r="D6" t="str">
-        <v>GENROU_5</v>
+        <v>GENROU_7</v>
       </c>
       <c r="E6" t="str">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" t="str">
-        <v>PV_5</v>
+        <v>PV_7</v>
       </c>
       <c r="G6" t="str">
         <v>COI_1</v>
       </c>
       <c r="H6" t="str">
-        <v>1080.2</v>
+        <v>1025.2</v>
       </c>
       <c r="I6" t="str">
-        <v>15.5</v>
+        <v>12.5</v>
       </c>
       <c r="J6" t="str">
         <v>60</v>
@@ -10214,16 +9557,16 @@
         <v>0</v>
       </c>
       <c r="L6" t="str">
-        <v>5.2</v>
+        <v>8.28</v>
       </c>
       <c r="M6" t="str">
-        <v>0.0014</v>
+        <v>0.00268</v>
       </c>
       <c r="N6" t="str">
-        <v>0.54</v>
+        <v>0.322</v>
       </c>
       <c r="O6" t="str">
-        <v>1.32</v>
+        <v>0.49</v>
       </c>
       <c r="P6" t="str">
         <v>0</v>
@@ -10238,28 +9581,28 @@
         <v>0</v>
       </c>
       <c r="T6" t="str">
-        <v>6.7</v>
+        <v>2.95</v>
       </c>
       <c r="U6" t="str">
-        <v>6.2</v>
+        <v>2.92</v>
       </c>
       <c r="V6" t="str">
-        <v>0.00571</v>
+        <v>0.02141</v>
       </c>
       <c r="W6" t="str">
-        <v>1.32</v>
+        <v>0.49</v>
       </c>
       <c r="X6" t="str">
-        <v>0.00571</v>
+        <v>0.02141</v>
       </c>
       <c r="Y6" t="str">
-        <v>5.4</v>
+        <v>5.66</v>
       </c>
       <c r="Z6" t="str">
         <v>0.03</v>
       </c>
       <c r="AA6" t="str">
-        <v>0.44</v>
+        <v>1.5</v>
       </c>
       <c r="AB6" t="str">
         <v>0.04</v>
@@ -10267,31 +9610,31 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" t="str">
-        <v>GENROU_6</v>
+        <v>GENROU_10</v>
       </c>
       <c r="C7" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="str">
-        <v>GENROU_6</v>
+        <v>GENROU_10</v>
       </c>
       <c r="E7" t="str">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F7" t="str">
-        <v>PV_6</v>
+        <v>Slack_10</v>
       </c>
       <c r="G7" t="str">
         <v>COI_1</v>
       </c>
       <c r="H7" t="str">
-        <v>1085.7</v>
+        <v>1199</v>
       </c>
       <c r="I7" t="str">
-        <v>15.5</v>
+        <v>345</v>
       </c>
       <c r="J7" t="str">
         <v>60</v>
@@ -10300,16 +9643,16 @@
         <v>0</v>
       </c>
       <c r="L7" t="str">
-        <v>6.96</v>
+        <v>10</v>
       </c>
       <c r="M7" t="str">
-        <v>0.0615</v>
+        <v>0.001</v>
       </c>
       <c r="N7" t="str">
-        <v>0.224</v>
+        <v>0.03</v>
       </c>
       <c r="O7" t="str">
-        <v>0.5</v>
+        <v>0.06</v>
       </c>
       <c r="P7" t="str">
         <v>0</v>
@@ -10324,387 +9667,43 @@
         <v>0</v>
       </c>
       <c r="T7" t="str">
-        <v>2.54</v>
+        <v>0.2</v>
       </c>
       <c r="U7" t="str">
-        <v>2.41</v>
+        <v>0.19</v>
       </c>
       <c r="V7" t="str">
-        <v>0.46538</v>
+        <v>0.0026</v>
       </c>
       <c r="W7" t="str">
-        <v>0.5</v>
+        <v>0.06</v>
       </c>
       <c r="X7" t="str">
-        <v>0.46538</v>
+        <v>0.0026</v>
       </c>
       <c r="Y7" t="str">
-        <v>7.3</v>
+        <v>7</v>
       </c>
       <c r="Z7" t="str">
         <v>0.03</v>
       </c>
       <c r="AA7" t="str">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="AB7" t="str">
         <v>0.04</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>6</v>
-      </c>
-      <c r="B8" t="str">
-        <v>GENROU_7</v>
-      </c>
-      <c r="C8" t="str">
-        <v>1</v>
-      </c>
-      <c r="D8" t="str">
-        <v>GENROU_7</v>
-      </c>
-      <c r="E8" t="str">
-        <v>36</v>
-      </c>
-      <c r="F8" t="str">
-        <v>PV_7</v>
-      </c>
-      <c r="G8" t="str">
-        <v>COI_1</v>
-      </c>
-      <c r="H8" t="str">
-        <v>1025.2</v>
-      </c>
-      <c r="I8" t="str">
-        <v>12.5</v>
-      </c>
-      <c r="J8" t="str">
-        <v>60</v>
-      </c>
-      <c r="K8" t="str">
-        <v>0</v>
-      </c>
-      <c r="L8" t="str">
-        <v>5.28</v>
-      </c>
-      <c r="M8" t="str">
-        <v>0.00268</v>
-      </c>
-      <c r="N8" t="str">
-        <v>0.322</v>
-      </c>
-      <c r="O8" t="str">
-        <v>0.49</v>
-      </c>
-      <c r="P8" t="str">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="str">
-        <v>0</v>
-      </c>
-      <c r="R8" t="str">
-        <v>0</v>
-      </c>
-      <c r="S8" t="str">
-        <v>0</v>
-      </c>
-      <c r="T8" t="str">
-        <v>2.95</v>
-      </c>
-      <c r="U8" t="str">
-        <v>2.92</v>
-      </c>
-      <c r="V8" t="str">
-        <v>0.02141</v>
-      </c>
-      <c r="W8" t="str">
-        <v>0.49</v>
-      </c>
-      <c r="X8" t="str">
-        <v>0.02141</v>
-      </c>
-      <c r="Y8" t="str">
-        <v>5.66</v>
-      </c>
-      <c r="Z8" t="str">
-        <v>0.03</v>
-      </c>
-      <c r="AA8" t="str">
-        <v>1.5</v>
-      </c>
-      <c r="AB8" t="str">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>7</v>
-      </c>
-      <c r="B9" t="str">
-        <v>GENROU_8</v>
-      </c>
-      <c r="C9" t="str">
-        <v>0</v>
-      </c>
-      <c r="D9" t="str">
-        <v>GENROU_8</v>
-      </c>
-      <c r="E9" t="str">
-        <v>37</v>
-      </c>
-      <c r="F9" t="str">
-        <v>PV_8</v>
-      </c>
-      <c r="G9" t="str">
-        <v>COI_1</v>
-      </c>
-      <c r="H9" t="str">
-        <v>970.2</v>
-      </c>
-      <c r="I9" t="str">
-        <v>12.5</v>
-      </c>
-      <c r="J9" t="str">
-        <v>60</v>
-      </c>
-      <c r="K9" t="str">
-        <v>0</v>
-      </c>
-      <c r="L9" t="str">
-        <v>4.86</v>
-      </c>
-      <c r="M9" t="str">
-        <v>0.00686</v>
-      </c>
-      <c r="N9" t="str">
-        <v>0.28</v>
-      </c>
-      <c r="O9" t="str">
-        <v>0.57</v>
-      </c>
-      <c r="P9" t="str">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="str">
-        <v>0</v>
-      </c>
-      <c r="R9" t="str">
-        <v>0</v>
-      </c>
-      <c r="S9" t="str">
-        <v>0</v>
-      </c>
-      <c r="T9" t="str">
-        <v>2.9</v>
-      </c>
-      <c r="U9" t="str">
-        <v>2.8</v>
-      </c>
-      <c r="V9" t="str">
-        <v>0.06076</v>
-      </c>
-      <c r="W9" t="str">
-        <v>0.57</v>
-      </c>
-      <c r="X9" t="str">
-        <v>0.06076</v>
-      </c>
-      <c r="Y9" t="str">
-        <v>6.7</v>
-      </c>
-      <c r="Z9" t="str">
-        <v>0.03</v>
-      </c>
-      <c r="AA9" t="str">
-        <v>0.41</v>
-      </c>
-      <c r="AB9" t="str">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>8</v>
-      </c>
-      <c r="B10" t="str">
-        <v>GENROU_9</v>
-      </c>
-      <c r="C10" t="str">
-        <v>0</v>
-      </c>
-      <c r="D10" t="str">
-        <v>GENROU_9</v>
-      </c>
-      <c r="E10" t="str">
-        <v>38</v>
-      </c>
-      <c r="F10" t="str">
-        <v>PV_9</v>
-      </c>
-      <c r="G10" t="str">
-        <v>COI_1</v>
-      </c>
-      <c r="H10" t="str">
-        <v>1684.1</v>
-      </c>
-      <c r="I10" t="str">
-        <v>34.5</v>
-      </c>
-      <c r="J10" t="str">
-        <v>60</v>
-      </c>
-      <c r="K10" t="str">
-        <v>0</v>
-      </c>
-      <c r="L10" t="str">
-        <v>6.9</v>
-      </c>
-      <c r="M10" t="str">
-        <v>0.003</v>
-      </c>
-      <c r="N10" t="str">
-        <v>0.298</v>
-      </c>
-      <c r="O10" t="str">
-        <v>0.57</v>
-      </c>
-      <c r="P10" t="str">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="str">
-        <v>0</v>
-      </c>
-      <c r="R10" t="str">
-        <v>0</v>
-      </c>
-      <c r="S10" t="str">
-        <v>0</v>
-      </c>
-      <c r="T10" t="str">
-        <v>2.106</v>
-      </c>
-      <c r="U10" t="str">
-        <v>2.05</v>
-      </c>
-      <c r="V10" t="str">
-        <v>0.01174</v>
-      </c>
-      <c r="W10" t="str">
-        <v>0.57</v>
-      </c>
-      <c r="X10" t="str">
-        <v>0.01174</v>
-      </c>
-      <c r="Y10" t="str">
-        <v>4.79</v>
-      </c>
-      <c r="Z10" t="str">
-        <v>0.03</v>
-      </c>
-      <c r="AA10" t="str">
-        <v>1.96</v>
-      </c>
-      <c r="AB10" t="str">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>9</v>
-      </c>
-      <c r="B11" t="str">
-        <v>GENROU_10</v>
-      </c>
-      <c r="C11" t="str">
-        <v>1</v>
-      </c>
-      <c r="D11" t="str">
-        <v>GENROU_10</v>
-      </c>
-      <c r="E11" t="str">
-        <v>39</v>
-      </c>
-      <c r="F11" t="str">
-        <v>Slack_10</v>
-      </c>
-      <c r="G11" t="str">
-        <v>COI_1</v>
-      </c>
-      <c r="H11" t="str">
-        <v>1199</v>
-      </c>
-      <c r="I11" t="str">
-        <v>345</v>
-      </c>
-      <c r="J11" t="str">
-        <v>60</v>
-      </c>
-      <c r="K11" t="str">
-        <v>0</v>
-      </c>
-      <c r="L11" t="str">
-        <v>100</v>
-      </c>
-      <c r="M11" t="str">
-        <v>0.001</v>
-      </c>
-      <c r="N11" t="str">
-        <v>0.03</v>
-      </c>
-      <c r="O11" t="str">
-        <v>0.06</v>
-      </c>
-      <c r="P11" t="str">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="str">
-        <v>0</v>
-      </c>
-      <c r="R11" t="str">
-        <v>0</v>
-      </c>
-      <c r="S11" t="str">
-        <v>0</v>
-      </c>
-      <c r="T11" t="str">
-        <v>0.2</v>
-      </c>
-      <c r="U11" t="str">
-        <v>0.19</v>
-      </c>
-      <c r="V11" t="str">
-        <v>0.0026</v>
-      </c>
-      <c r="W11" t="str">
-        <v>0.06</v>
-      </c>
-      <c r="X11" t="str">
-        <v>0.0026</v>
-      </c>
-      <c r="Y11" t="str">
-        <v>7</v>
-      </c>
-      <c r="Z11" t="str">
-        <v>0.03</v>
-      </c>
-      <c r="AA11" t="str">
-        <v>0.7</v>
-      </c>
-      <c r="AB11" t="str">
-        <v>0.04</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AB11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AB7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10824,34 +9823,34 @@
         <v>0</v>
       </c>
       <c r="M2" t="str">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N2" t="str">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O2" t="str">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="P2" t="str">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="str">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="R2" t="str">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S2" t="str">
         <v>500</v>
       </c>
       <c r="T2" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U2" t="str">
         <v>500</v>
       </c>
       <c r="V2" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W2" t="str">
         <v>0</v>
@@ -10904,31 +9903,31 @@
         <v>6</v>
       </c>
       <c r="N3" t="str">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O3" t="str">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="P3" t="str">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="str">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="R3" t="str">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S3" t="str">
         <v>500</v>
       </c>
       <c r="T3" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U3" t="str">
         <v>500</v>
       </c>
       <c r="V3" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W3" t="str">
         <v>0</v>
@@ -10978,34 +9977,34 @@
         <v>0</v>
       </c>
       <c r="M4" t="str">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N4" t="str">
         <v>3</v>
       </c>
       <c r="O4" t="str">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="P4" t="str">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="str">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="R4" t="str">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S4" t="str">
         <v>500</v>
       </c>
       <c r="T4" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U4" t="str">
         <v>500</v>
       </c>
       <c r="V4" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W4" t="str">
         <v>0</v>
@@ -11058,31 +10057,31 @@
         <v>6</v>
       </c>
       <c r="N5" t="str">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O5" t="str">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="P5" t="str">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="str">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="R5" t="str">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S5" t="str">
         <v>500</v>
       </c>
       <c r="T5" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="U5" t="str">
         <v>500</v>
       </c>
       <c r="V5" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="W5" t="str">
         <v>0</v>
@@ -11097,9 +10096,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="U7" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Z5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Z7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
solve the problem of andes Sbase
</commit_message>
<xml_diff>
--- a/bshe/VIS_opf/ieee39_vis.xlsx
+++ b/bshe/VIS_opf/ieee39_vis.xlsx
@@ -3865,7 +3865,7 @@
         <v>Toggler_1</v>
       </c>
       <c r="C2" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="str">
         <v>Toggler_1</v>
@@ -3877,29 +3877,6 @@
         <v>GENROU_2</v>
       </c>
       <c r="G2" t="str">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>1</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Toggler_2</v>
-      </c>
-      <c r="C3" t="str">
-        <v>1</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Toggler_1</v>
-      </c>
-      <c r="E3" t="str">
-        <v>PQ</v>
-      </c>
-      <c r="F3" t="str">
-        <v>PQ_20</v>
-      </c>
-      <c r="G3" t="str">
         <v>5</v>
       </c>
     </row>
@@ -3959,7 +3936,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4664,44 +4641,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>19</v>
-      </c>
-      <c r="B21" t="str">
-        <v>PQ_20</v>
-      </c>
-      <c r="C21" t="str">
-        <v>0</v>
-      </c>
-      <c r="D21" t="str">
-        <v>PQ_18</v>
-      </c>
-      <c r="E21" t="str">
-        <v>31</v>
-      </c>
-      <c r="F21" t="str">
-        <v>34.5</v>
-      </c>
-      <c r="G21" t="str">
-        <v>0.8</v>
-      </c>
-      <c r="H21" t="str">
-        <v>0.4</v>
-      </c>
-      <c r="I21" t="str">
-        <v>1.2</v>
-      </c>
-      <c r="J21" t="str">
-        <v>0.8</v>
-      </c>
-      <c r="K21" t="str">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K20"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9210,7 +9152,7 @@
         <v>60</v>
       </c>
       <c r="K2" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="str">
         <v>8.06</v>
@@ -9296,7 +9238,7 @@
         <v>60</v>
       </c>
       <c r="K3" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" t="str">
         <v>7.16</v>
@@ -9382,7 +9324,7 @@
         <v>60</v>
       </c>
       <c r="K4" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="str">
         <v>8.72</v>
@@ -9468,7 +9410,7 @@
         <v>60</v>
       </c>
       <c r="K5" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="str">
         <v>5.2</v>
@@ -9554,7 +9496,7 @@
         <v>60</v>
       </c>
       <c r="K6" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" t="str">
         <v>8.28</v>
@@ -9640,7 +9582,7 @@
         <v>60</v>
       </c>
       <c r="K7" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" t="str">
         <v>10</v>

</xml_diff>

<commit_message>
clean vis1 and vis2, add note
</commit_message>
<xml_diff>
--- a/bshe/VIS_opf/ieee39_vis.xlsx
+++ b/bshe/VIS_opf/ieee39_vis.xlsx
@@ -4746,7 +4746,7 @@
         <v>15</v>
       </c>
       <c r="L2" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M2" t="str">
         <v>1.83816</v>
@@ -5026,7 +5026,7 @@
         <v>8</v>
       </c>
       <c r="L7" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" t="str">
         <v>7.125456</v>
@@ -5138,7 +5138,7 @@
         <v>7</v>
       </c>
       <c r="L9" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" t="str">
         <v>5.321616</v>
@@ -5194,7 +5194,7 @@
         <v>10</v>
       </c>
       <c r="L10" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" t="str">
         <v>10.0173</v>

</xml_diff>

<commit_message>
draft TDS for visopf, add code note
</commit_message>
<xml_diff>
--- a/bshe/VIS_opf/ieee39_vis.xlsx
+++ b/bshe/VIS_opf/ieee39_vis.xlsx
@@ -9735,7 +9735,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>1</v>
+        <v>VSG_1</v>
       </c>
       <c r="C2" t="str">
         <v>1</v>
@@ -9812,7 +9812,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>2</v>
+        <v>VSG_2</v>
       </c>
       <c r="C3" t="str">
         <v>1</v>
@@ -9889,7 +9889,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>3</v>
+        <v>VSG_3</v>
       </c>
       <c r="C4" t="str">
         <v>1</v>
@@ -9966,7 +9966,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>4</v>
+        <v>VSG_4</v>
       </c>
       <c r="C5" t="str">
         <v>1</v>

</xml_diff>